<commit_message>
AIP-629 AIP-640 Added Test Data Files
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_18Channel/1U3I3I3I3I.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_18Channel/1U3I3I3I3I.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D98625F-97EC-476A-AF90-53B54DF4C1F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146D1B38-FAEA-42EC-BC70-218B767833C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -449,9 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -771,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFEAB912-4FA8-45F1-A838-D38ED09FB262}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -781,58 +779,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>-1</v>
       </c>
     </row>
@@ -856,135 +854,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>98</v>
       </c>
       <c r="B17">
@@ -992,7 +990,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>99</v>
       </c>
       <c r="B18">
@@ -1000,7 +998,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>100</v>
       </c>
       <c r="B19">
@@ -1008,7 +1006,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>101</v>
       </c>
       <c r="B20">
@@ -1016,7 +1014,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>102</v>
       </c>
       <c r="B21">
@@ -1024,7 +1022,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>103</v>
       </c>
       <c r="B22">
@@ -1032,7 +1030,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>104</v>
       </c>
       <c r="B23">
@@ -1040,7 +1038,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>105</v>
       </c>
       <c r="B24">
@@ -1048,7 +1046,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>106</v>
       </c>
       <c r="B25">
@@ -1056,7 +1054,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>107</v>
       </c>
       <c r="B26">
@@ -1064,7 +1062,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>108</v>
       </c>
       <c r="B27">
@@ -1072,7 +1070,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>109</v>
       </c>
       <c r="B28">
@@ -1080,7 +1078,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>110</v>
       </c>
       <c r="B29">
@@ -1088,7 +1086,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>111</v>
       </c>
       <c r="B30">
@@ -1096,7 +1094,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>112</v>
       </c>
       <c r="B31">
@@ -1104,7 +1102,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>113</v>
       </c>
       <c r="B32">
@@ -1112,7 +1110,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>114</v>
       </c>
       <c r="B33">
@@ -1120,7 +1118,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>115</v>
       </c>
       <c r="B34">
@@ -1128,7 +1126,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>116</v>
       </c>
       <c r="B35">
@@ -1136,7 +1134,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>117</v>
       </c>
       <c r="B36">
@@ -1144,7 +1142,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>118</v>
       </c>
       <c r="B37">
@@ -1152,7 +1150,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>119</v>
       </c>
       <c r="B38">
@@ -1160,7 +1158,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>120</v>
       </c>
       <c r="B39">
@@ -1168,7 +1166,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>121</v>
       </c>
       <c r="B40">
@@ -1176,7 +1174,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>122</v>
       </c>
       <c r="B41">
@@ -1193,8 +1191,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>